<commit_message>
Code updated 23-02-04 11:31:00
</commit_message>
<xml_diff>
--- a/Season_Trophies/83.xlsx
+++ b/Season_Trophies/83.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E159"/>
+  <dimension ref="A1:E160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20026</t>
+          <t>23573</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -416,14 +416,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>3409</t>
+          <t>3422</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>259</t>
+          <t>288</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -443,14 +443,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4750</t>
+          <t>5035</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7506</t>
+          <t>7299</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -470,14 +470,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3949</t>
+          <t>4181</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>783</t>
+          <t>874</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -497,14 +497,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4576</t>
+          <t>4861</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1244</t>
+          <t>1217</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -524,14 +524,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4490</t>
+          <t>4787</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1519</t>
+          <t>2894</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -551,14 +551,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4444</t>
+          <t>4544</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>7139</t>
+          <t>4318</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -578,14 +578,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>3970</t>
+          <t>4415</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>7669</t>
+          <t>7290</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -605,14 +605,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3940</t>
+          <t>4181</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>7986</t>
+          <t>11163</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -632,14 +632,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>3922</t>
+          <t>3950</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>10250</t>
+          <t>13974</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -659,24 +659,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3800</t>
+          <t>3803</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>249</t>
+          <t>305</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>27484940</t>
+          <t>8741713</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Auto-Battle</t>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -686,24 +686,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4757</t>
+          <t>5029</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>421</t>
+          <t>535</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>8741713</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve">㊥大咖玩家ky </t>
+          <t>"落日幻影 哈哈哈"</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4680</t>
+          <t>4950</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>880</t>
+          <t>892</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>25376635</t>
+          <t>31267627</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"sanchez ᶻᵍˣ"</t>
+          <t>"㊥ Martin"</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>4555</t>
+          <t>4857</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1024</t>
+          <t>1393</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>31267627</t>
+          <t>29211638</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>"㊥ Martin"</t>
+          <t>"㊥ PhononDisperse"</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4525</t>
+          <t>4751</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1095</t>
+          <t>2300</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>27484940</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>"落日幻影 哈哈哈"</t>
+          <t>Auto-Battle</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>4513</t>
+          <t>4611</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1314</t>
+          <t>2324</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>27468237</t>
+          <t>3946814</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>佛系复仇者秀川</t>
+          <t>"小瑩 潘"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4479</t>
+          <t>4608</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1557</t>
+          <t>2442</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>29211638</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>"㊥ PhononDisperse"</t>
+          <t>Kikkik</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>4437</t>
+          <t>4596</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1736</t>
+          <t>2476</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>21735478</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Kikkik</t>
+          <t>耀翔fly</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4412</t>
+          <t>4594</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2696</t>
+          <t>2588</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3946814</t>
+          <t>27468237</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"小瑩 潘"</t>
+          <t>佛系复仇者秀川</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>4299</t>
+          <t>4581</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3149</t>
+          <t>2745</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>9913517</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>"Kenny Chan"</t>
+          <t>kusipao</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,24 +929,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4257</t>
+          <t>4561</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3519</t>
+          <t>2834</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>26588375</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>kusipao</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>4224</t>
+          <t>4549</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4248</t>
+          <t>3429</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>30411791</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>4164</t>
+          <t>4493</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4332</t>
+          <t>4317</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>21735478</t>
+          <t>28387448</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>耀翔fly</t>
+          <t>☜⊙‖⊙☞</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4157</t>
+          <t>4415</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4481</t>
+          <t>4475</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1820342</t>
+          <t>29729468</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>摸鱼者三战</t>
+          <t>"风神舞动 WDᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4145</t>
+          <t>4401</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5144</t>
+          <t>5073</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>29729468</t>
+          <t>1820342</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>"风神舞动 WDᶻᵍˣ"</t>
+          <t>摸鱼者三战</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,14 +1064,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>4099</t>
+          <t>4354</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5367</t>
+          <t>5097</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4084</t>
+          <t>4352</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5387</t>
+          <t>5215</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>33656016</t>
+          <t>30411791</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>㊥☆梅海听雪☆</t>
+          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,14 +1118,14 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4083</t>
+          <t>4343</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5491</t>
+          <t>5228</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1145,14 +1145,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>4075</t>
+          <t>4342</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5570</t>
+          <t>5222</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4069</t>
+          <t>4342</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5879</t>
+          <t>5402</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>21345373</t>
+          <t>3477306</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>林北不講武德</t>
+          <t>"MeGa Tsai"</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>4047</t>
+          <t>4325</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5972</t>
+          <t>5457</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>28387448</t>
+          <t>21345373</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>☜⊙‖⊙☞</t>
+          <t>林北不講武德</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4041</t>
+          <t>4321</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6354</t>
+          <t>5979</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16206490</t>
+          <t>33656016</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>㊥Godcys</t>
+          <t>㊥☆梅海听雪☆</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4017</t>
+          <t>4282</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6595</t>
+          <t>6056</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3477306</t>
+          <t>16206490</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>"MeGa Tsai"</t>
+          <t>㊥Godcys</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,14 +1280,14 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4001</t>
+          <t>4275</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>7645</t>
+          <t>7203</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>3941</t>
+          <t>4188</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>8192</t>
+          <t>7767</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4229136</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>"totoro wu"</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>3910</t>
+          <t>4149</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>9536</t>
+          <t>7907</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>29861826</t>
+          <t>4229136</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>★★★Eric★★★</t>
+          <t>"totoro wu"</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>3837</t>
+          <t>4139</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>10143</t>
+          <t>9955</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>27113069</t>
+          <t>29861826</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>㊥DumbSmoky</t>
+          <t>★★★Eric★★★</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3806</t>
+          <t>4013</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>10260</t>
+          <t>10077</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>27113069</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>㊥DumbSmoky</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,14 +1415,14 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3799</t>
+          <t>4007</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>11177</t>
+          <t>10414</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>3755</t>
+          <t>3989</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>11385</t>
+          <t>10596</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7025661</t>
+          <t>44955827</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"F ᶻᵍˣ"</t>
+          <t>丶小阿狸丿</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,24 +1469,24 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>3744</t>
+          <t>3980</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>11823</t>
+          <t>11822</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>44955827</t>
+          <t>7025661</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>丶小阿狸丿</t>
+          <t>"F ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1496,14 +1496,14 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>3724</t>
+          <t>3917</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>14959</t>
+          <t>14506</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1523,14 +1523,14 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>3590</t>
+          <t>3780</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>18250</t>
+          <t>16704</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1550,14 +1550,14 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>3469</t>
+          <t>3683</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>19089</t>
+          <t>19198</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1577,24 +1577,24 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>3441</t>
+          <t>3587</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>30013</t>
+          <t>26554</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1604,24 +1604,24 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>3100</t>
+          <t>3316</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>32226</t>
+          <t>33537</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1631,24 +1631,24 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>3037</t>
+          <t>3100</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>39059</t>
+          <t>35659</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>21665473</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>"Dog Gamedesiger"</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1658,14 +1658,14 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>2868</t>
+          <t>3037</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>48450</t>
+          <t>49357</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1685,7 +1685,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2657</t>
+          <t>2686</t>
         </is>
       </c>
     </row>
@@ -1719,7 +1719,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>15661</t>
+          <t>16584</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1739,14 +1739,14 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>3563</t>
+          <t>3688</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20100</t>
+          <t>18461</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>3406</t>
+          <t>3614</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6703</t>
+          <t>5900</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>13738844</t>
+          <t>28749280</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>"Chen Hao"</t>
+          <t>㊥老船⛵⛵</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>3995</t>
+          <t>4287</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>7200</t>
+          <t>6708</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>28749280</t>
+          <t>13738844</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>㊥老船⛵⛵</t>
+          <t>"Chen Hao"</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,14 +1820,14 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>3966</t>
+          <t>4226</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>9884</t>
+          <t>9538</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1847,14 +1847,14 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>3818</t>
+          <t>4037</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>10522</t>
+          <t>10462</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1874,14 +1874,14 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>3787</t>
+          <t>3986</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>13396</t>
+          <t>11299</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1901,14 +1901,14 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>3655</t>
+          <t>3944</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>17900</t>
+          <t>17137</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1928,14 +1928,14 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3480</t>
+          <t>3666</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>40332</t>
+          <t>38753</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>2838</t>
+          <t>2954</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>4245</t>
+          <t>4897</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>心灵有为</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>4164</t>
+          <t>4368</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5001</t>
+          <t>5049</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>38711610</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>4108</t>
+          <t>4355</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6656</t>
+          <t>6612</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>3997</t>
+          <t>4234</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>8013</t>
+          <t>8498</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>3920</t>
+          <t>4100</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>8787</t>
+          <t>9747</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>22885399</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>余文琪</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,14 +2090,14 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>3877</t>
+          <t>4025</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>8663</t>
+          <t>10175</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>3884</t>
+          <t>4001</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>9838</t>
+          <t>10153</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>22885399</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>余文琪</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>3821</t>
+          <t>4003</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>11813</t>
+          <t>11803</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>42434117</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>㊥有双飞鸟</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>3725</t>
+          <t>3918</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>12257</t>
+          <t>12918</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>42434117</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>㊥有双飞鸟</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,14 +2198,14 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>3706</t>
+          <t>3859</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>16724</t>
+          <t>16551</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2225,14 +2225,14 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>3521</t>
+          <t>3689</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>18150</t>
+          <t>17982</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2252,14 +2252,14 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>3472</t>
+          <t>3634</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>19126</t>
+          <t>19843</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2279,14 +2279,14 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>3439</t>
+          <t>3561</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>23349</t>
+          <t>20703</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2306,14 +2306,14 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>3296</t>
+          <t>3530</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>24938</t>
+          <t>23811</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -2333,14 +2333,14 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>3246</t>
+          <t>3412</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>25042</t>
+          <t>23977</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>3243</t>
+          <t>3406</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>36437</t>
+          <t>35718</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>22161051</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>Botz5</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>2930</t>
+          <t>3036</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>37283</t>
+          <t>38001</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>22161051</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Botz5</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,14 +2414,14 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>2909</t>
+          <t>2975</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>36931</t>
+          <t>38758</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2441,14 +2441,14 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>2917</t>
+          <t>2954</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>43675</t>
+          <t>40641</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2468,14 +2468,14 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>2762</t>
+          <t>2902</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>43693</t>
+          <t>43786</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2495,14 +2495,14 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>2761</t>
+          <t>2820</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>44828</t>
+          <t>44731</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2522,14 +2522,14 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>2735</t>
+          <t>2796</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>45283</t>
+          <t>46492</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2549,14 +2549,14 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>2725</t>
+          <t>2753</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>45846</t>
+          <t>47500</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>2714</t>
+          <t>2729</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>46911</t>
+          <t>48534</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>57813281</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>XAUEN</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,24 +2603,24 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>2690</t>
+          <t>2704</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>50014</t>
+          <t>49244</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>68132</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>"㊖TW9 百媚生"</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>2628</t>
+          <t>2688</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>51022</t>
+          <t>50347</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>14110169</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>"Pasiony CANQ"</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,24 +2657,24 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>2609</t>
+          <t>2664</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>52678</t>
+          <t>53030</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>57813281</t>
+          <t>14110169</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>XAUEN</t>
+          <t>"Pasiony CANQ"</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2684,14 +2684,14 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2579</t>
+          <t>2609</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>54781</t>
+          <t>56612</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2718,7 +2718,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>58730</t>
+          <t>60186</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2772,7 +2772,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>53721</t>
+          <t>55545</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2799,17 +2799,17 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>15159</t>
+          <t>15494</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>25163202</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>"sam yang"</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2819,24 +2819,24 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>3583</t>
+          <t>3736</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>16181</t>
+          <t>16088</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>25163202</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>"sam yang"</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2846,14 +2846,14 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>3542</t>
+          <t>3709</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>16841</t>
+          <t>18388</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2873,24 +2873,24 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>3517</t>
+          <t>3617</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>25464</t>
+          <t>25225</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,14 +2900,14 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>3230</t>
+          <t>3363</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>26122</t>
+          <t>26020</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>3212</t>
+          <t>3335</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>26623</t>
+          <t>25617</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,14 +2954,14 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>3198</t>
+          <t>3350</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>27453</t>
+          <t>26631</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2981,14 +2981,14 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>3174</t>
+          <t>3313</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>39017</t>
+          <t>42255</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>2869</t>
+          <t>2861</t>
         </is>
       </c>
     </row>
@@ -3042,7 +3042,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>25039</t>
+          <t>26514</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>3243</t>
+          <t>3317</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>30025</t>
+          <t>27650</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>3099</t>
+          <t>3282</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>29622</t>
+          <t>28488</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>3110</t>
+          <t>3255</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>30764</t>
+          <t>28701</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,14 +3143,14 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>3079</t>
+          <t>3248</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>34603</t>
+          <t>34063</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>2977</t>
+          <t>3084</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>34928</t>
+          <t>36928</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,14 +3197,14 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>2969</t>
+          <t>3001</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>37752</t>
+          <t>35672</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>2898</t>
+          <t>3036</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>37979</t>
+          <t>37387</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,14 +3251,14 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>2893</t>
+          <t>2991</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>38792</t>
+          <t>38637</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>2874</t>
+          <t>2957</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>38791</t>
+          <t>39302</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,14 +3305,14 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>2874</t>
+          <t>2938</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>42141</t>
+          <t>43162</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -3332,14 +3332,14 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>2795</t>
+          <t>2836</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>46370</t>
+          <t>45511</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>2702</t>
+          <t>2777</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>47645</t>
+          <t>46597</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>55499394</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Player-55499394</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>2675</t>
+          <t>2751</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>49310</t>
+          <t>48084</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>2642</t>
+          <t>2715</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>53216</t>
+          <t>50375</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>55499394</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>Player-55499394</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,14 +3440,14 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>2571</t>
+          <t>2663</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>51957</t>
+          <t>51483</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>2591</t>
+          <t>2638</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>54297</t>
+          <t>52748</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>2554</t>
+          <t>2614</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>55567</t>
+          <t>56217</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>2537</t>
+          <t>2553</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>56330</t>
+          <t>57682</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>52792063</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>"Tramaine Dowlen"</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>2527</t>
+          <t>2531</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>60047</t>
+          <t>58022</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>1304123</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>Cccccccccccc</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,24 +3575,24 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>2490</t>
+          <t>2527</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>62966</t>
+          <t>62904</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>2454</t>
+          <t>2472</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>65364</t>
+          <t>64591</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,24 +3629,24 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>2417</t>
+          <t>2447</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>66056</t>
+          <t>67166</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Player-20372140</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>2405</t>
+          <t>2399</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>69061</t>
+          <t>67866</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Player-20372140</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,14 +3683,14 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>2313</t>
+          <t>2383</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>74911</t>
+          <t>69127</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3710,24 +3710,24 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>2126</t>
+          <t>2346</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>77909</t>
+          <t>70108</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>15436348</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3737,24 +3737,24 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>2067</t>
+          <t>2310</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>77842</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3764,7 +3764,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2100</t>
         </is>
       </c>
     </row>
@@ -3776,12 +3776,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -3803,12 +3803,12 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3825,44 +3825,44 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>49945</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>二馆</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2629</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>29386</t>
+          <t>50468</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3872,24 +3872,24 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>3117</t>
+          <t>2661</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>45635</t>
+          <t>34498</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3899,24 +3899,24 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>2718</t>
+          <t>3072</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>50835</t>
+          <t>45033</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3926,24 +3926,24 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>2612</t>
+          <t>2789</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>59923</t>
+          <t>51843</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>57219176</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>青莲道人</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>2491</t>
+          <t>2631</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>68957</t>
+          <t>61442</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>57219176</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>青莲道人</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,24 +3980,24 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>2317</t>
+          <t>2490</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>73596</t>
+          <t>67916</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>58739336</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Player-58739336</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,24 +4007,24 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>2163</t>
+          <t>2381</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>76275</t>
+          <t>69016</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>47533851</t>
+          <t>58739336</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Bibek</t>
+          <t>Player-58739336</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4034,24 +4034,24 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>2095</t>
+          <t>2350</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>89743</t>
+          <t>77440</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>58689512</t>
+          <t>47533851</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Player-58689512</t>
+          <t>Bibek</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4061,24 +4061,24 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>1817</t>
+          <t>2108</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>95248</t>
+          <t>91235</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>58644547</t>
+          <t>58689512</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>RotaryPreparation39</t>
+          <t>Player-58689512</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4088,24 +4088,24 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>1611</t>
+          <t>1817</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>103476</t>
+          <t>97492</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>58739866</t>
+          <t>58644547</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Player-58739866</t>
+          <t>RotaryPreparation39</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4115,14 +4115,14 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>1508</t>
+          <t>1611</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>104386</t>
+          <t>107004</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -4149,17 +4149,17 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>130643</t>
+          <t>112878</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>46248210</t>
+          <t>58739866</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Ajay</t>
+          <t>Player-58739866</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4169,24 +4169,24 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>1199</t>
+          <t>1480</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>137394</t>
+          <t>135126</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>57339836</t>
+          <t>46248210</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Player-57339836</t>
+          <t>Ajay</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,24 +4196,24 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1199</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>142784</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>57722377</t>
+          <t>57339836</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>VI空白IV</t>
+          <t>Player-57339836</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1100</t>
         </is>
       </c>
     </row>
@@ -4235,12 +4235,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>57867293</t>
+          <t>57722377</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Player-57867293</t>
+          <t>VI空白IV</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4262,12 +4262,12 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>57867293</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>Player-57867293</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4289,12 +4289,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>54924790</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Sujit4u</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4316,12 +4316,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>58132159</t>
+          <t>54924790</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>ExultantDelivery42</t>
+          <t>Sujit4u</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4343,12 +4343,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>55963040</t>
+          <t>58132159</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Baliram</t>
+          <t>ExultantDelivery42</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4370,12 +4370,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>53269862</t>
+          <t>55963040</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>New_Player111</t>
+          <t>Baliram</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4397,12 +4397,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>58562596</t>
+          <t>53269862</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Player-58562596</t>
+          <t>New_Player111</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4424,12 +4424,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>50742014</t>
+          <t>58562596</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>"Aditya Naik"</t>
+          <t>Player-58562596</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4451,12 +4451,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>58705573</t>
+          <t>50742014</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Player-58705573</t>
+          <t>"Aditya Naik"</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4473,44 +4473,44 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>48383</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>58705573</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>Player-58705573</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>2659</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>11500</t>
+          <t>46258</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4520,24 +4520,24 @@
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>3738</t>
+          <t>2759</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>44470</t>
+          <t>14634</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -4547,24 +4547,24 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>2744</t>
+          <t>3773</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>44547</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -4574,7 +4574,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2801</t>
         </is>
       </c>
     </row>
@@ -4586,12 +4586,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -4613,12 +4613,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -4640,20 +4640,47 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
+          <t>8850180</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>30624300</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
           <t>28624723</t>
         </is>
       </c>
-      <c r="C159" t="inlineStr">
+      <c r="C160" t="inlineStr">
         <is>
           <t>"Woody Shade"</t>
         </is>
       </c>
-      <c r="D159" t="inlineStr">
+      <c r="D160" t="inlineStr">
         <is>
           <t>Chinese</t>
         </is>
       </c>
-      <c r="E159" t="inlineStr">
+      <c r="E160" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-02-13 11:30:38
</commit_message>
<xml_diff>
--- a/Season_Trophies/83.xlsx
+++ b/Season_Trophies/83.xlsx
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>26066</t>
+          <t>20931</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -416,24 +416,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4009</t>
+          <t>4553</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>309</t>
+          <t>1810</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26424998</t>
+          <t>22497</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>"Smok3y Is Back"</t>
+          <t>xixihahagggᶻᵍˣ</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -443,24 +443,24 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>6813</t>
+          <t>6850</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1250</t>
+          <t>3820</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>27484940</t>
+          <t>1820342</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Auto-Battle</t>
+          <t>摸鱼者三战</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -470,24 +470,24 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>6475</t>
+          <t>6385</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>8803</t>
+          <t>2776</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>31217211</t>
+          <t>1951758</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>解憂雜貨鋪㊥</t>
+          <t>我來找你了</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -497,24 +497,24 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5242</t>
+          <t>6590</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>943</t>
+          <t>4209</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>32613475</t>
+          <t>3477306</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>"李 无 善 德"</t>
+          <t>"MeGa Tsai"</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -524,24 +524,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6566</t>
+          <t>6319</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1286</t>
+          <t>1315</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>6940556</t>
+          <t>3946814</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
+          <t>"小瑩 潘"</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -551,24 +551,24 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6465</t>
+          <t>7022</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1932</t>
+          <t>7583</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>22497</t>
+          <t>4229136</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>xixihahagggᶻᵍˣ</t>
+          <t>"totoro wu"</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -578,24 +578,24 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>6294</t>
+          <t>5762</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2746</t>
+          <t>6427</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11783968</t>
+          <t>6510348</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>F---119</t>
+          <t>Bonpoisson</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -605,24 +605,24 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>6114</t>
+          <t>6023</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3566</t>
+          <t>397</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>43800641</t>
+          <t>6940556</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>㊥蛋蛋大</t>
+          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -632,24 +632,24 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5969</t>
+          <t>7337</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>971</t>
+          <t>5066</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>47928278</t>
+          <t>7025661</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>"落日幻影 哈哈哈"</t>
+          <t>"F ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -659,24 +659,24 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>6558</t>
+          <t>6186</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1334</t>
+          <t>54752</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>31267627</t>
+          <t>7587898</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>"㊥ Martin"</t>
+          <t>藍精靈ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -686,24 +686,24 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>6451</t>
+          <t>2839</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2446</t>
+          <t>1099</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>25376635</t>
+          <t>8741713</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>"sanchez ᶻᵍˣ"</t>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -713,24 +713,24 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>6177</t>
+          <t>7055</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2889</t>
+          <t>4919</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>9913517</t>
+          <t>9541747</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>"Kenny Chan"</t>
+          <t>豹子头林冲</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -740,24 +740,24 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>6085</t>
+          <t>6207</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3202</t>
+          <t>3441</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>24733875</t>
+          <t>9913517</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Kikkik</t>
+          <t>"Kenny Chan"</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -767,24 +767,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>6028</t>
+          <t>6450</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3348</t>
+          <t>2371</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1951758</t>
+          <t>11783968</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>我來找你了</t>
+          <t>F---119</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -794,24 +794,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>6006</t>
+          <t>6690</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3442</t>
+          <t>16207</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>27468237</t>
+          <t>12333251</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>佛系复仇者秀川</t>
+          <t>"㊌ Mingxuan"</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -821,24 +821,24 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>5991</t>
+          <t>4833</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3861</t>
+          <t>12104</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>28387448</t>
+          <t>14424176</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>☜⊙‖⊙☞</t>
+          <t>天才少年老纪</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -848,24 +848,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>5917</t>
+          <t>5241</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3918</t>
+          <t>4709</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>21735478</t>
+          <t>16206490</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>耀翔fly</t>
+          <t>㊥Godcys</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -875,24 +875,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>5909</t>
+          <t>6239</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4633</t>
+          <t>618</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>3477306</t>
+          <t>20199374</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>"MeGa Tsai"</t>
+          <t>RuanFan</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -902,24 +902,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>5810</t>
+          <t>7293</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4755</t>
+          <t>8685</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>44955827</t>
+          <t>20737010</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>丶小阿狸丿</t>
+          <t>混着玩...</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -929,14 +929,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>5795</t>
+          <t>5586</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4828</t>
+          <t>4279</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -956,24 +956,24 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>5786</t>
+          <t>6304</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4952</t>
+          <t>4799</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>6510348</t>
+          <t>21665473</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bonpoisson</t>
+          <t>"Dog Gamedesiger"</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -983,24 +983,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>5768</t>
+          <t>6225</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>5023</t>
+          <t>3015</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>33656016</t>
+          <t>21735478</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>㊥☆梅海听雪☆</t>
+          <t>耀翔fly</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1010,24 +1010,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>5759</t>
+          <t>6540</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>5412</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>30411791</t>
+          <t>23687250</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
+          <t>"jetlijp ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1037,24 +1037,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>5703</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>5442</t>
+          <t>4166</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>29729468</t>
+          <t>24733875</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>"风神舞动 WDᶻᵍˣ"</t>
+          <t>Kikkik</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1064,24 +1064,24 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>5700</t>
+          <t>6322</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>5699</t>
+          <t>3045</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>32478707</t>
+          <t>25376635</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>"Bt So"</t>
+          <t>"sanchez ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1091,24 +1091,24 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>5668</t>
+          <t>6544</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>6272</t>
+          <t>3835</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1820342</t>
+          <t>26280580</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>摸鱼者三战</t>
+          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1118,24 +1118,24 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>5590</t>
+          <t>6382</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6363</t>
+          <t>672</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>26280580</t>
+          <t>26424998</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>꧁S.TIGRESS꧂ᶻᵍˣ</t>
+          <t>"Smok3y Is Back"</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1145,24 +1145,24 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5578</t>
+          <t>7216</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>6461</t>
+          <t>7477</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>21665473</t>
+          <t>27113069</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>"Dog Gamedesiger"</t>
+          <t>㊥DumbSmoky</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1172,24 +1172,24 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>5563</t>
+          <t>5792</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>9017</t>
+          <t>2111</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4229136</t>
+          <t>27468237</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>"totoro wu"</t>
+          <t>佛系复仇者秀川</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1199,24 +1199,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>5219</t>
+          <t>6760</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>9716</t>
+          <t>1234</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>27113069</t>
+          <t>27484940</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>㊥DumbSmoky</t>
+          <t>66666zgx</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1226,24 +1226,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>5147</t>
+          <t>7026</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>12028</t>
+          <t>5424</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>29861826</t>
+          <t>28387448</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>★★★Eric★★★</t>
+          <t>☜⊙‖⊙☞</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1253,24 +1253,24 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4942</t>
+          <t>6140</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>12710</t>
+          <t>4104</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>14424176</t>
+          <t>28749280</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>天才少年老纪</t>
+          <t>㊥老船⛵⛵</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1280,24 +1280,24 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>4881</t>
+          <t>6334</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>13741</t>
+          <t>1546</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>47146736</t>
+          <t>29211638</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>"HK 品瑜"</t>
+          <t>"㊥ PhononDisperse"</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1307,24 +1307,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4789</t>
+          <t>6934</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>15428</t>
+          <t>4356</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>12333251</t>
+          <t>29729468</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>"㊌ Mingxuan"</t>
+          <t>"风神舞动 WDᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1334,24 +1334,24 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4656</t>
+          <t>6305</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>17284</t>
+          <t>13726</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>20737010</t>
+          <t>29861826</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>混着玩...</t>
+          <t>★★★Eric★★★</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1361,24 +1361,24 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4530</t>
+          <t>5062</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>46088</t>
+          <t>4427</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>57551884</t>
+          <t>30411791</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>|maaz|</t>
+          <t>"㊥Ⓩ GOÐAFRÆÐI ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1388,24 +1388,24 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>3113</t>
+          <t>6293</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>47927</t>
+          <t>5456</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>45967307</t>
+          <t>31217211</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Ricky</t>
+          <t>解憂雜貨鋪㊥</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1415,24 +1415,24 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>3035</t>
+          <t>6135</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>52935</t>
+          <t>989</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>7587898</t>
+          <t>31267627</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>藍精靈ᶻᵍˣ</t>
+          <t>"㊥ Martin"</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1442,24 +1442,24 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2840</t>
+          <t>7146</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>6965</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>23687250</t>
+          <t>32478707</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>"jetlijp ᶻᵍˣ"</t>
+          <t>"Bt So"</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1469,267 +1469,267 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5908</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20964</t>
+          <t>703</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>37861953</t>
+          <t>32613475</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>"Durex ๑• . •๑"</t>
+          <t>"李 无 善 德"</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>4314</t>
+          <t>7214</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>19309</t>
+          <t>5246</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>38809086</t>
+          <t>33656016</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Kouenᶻᵍˣ</t>
+          <t>㊥☆梅海听雪☆</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>4410</t>
+          <t>6162</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4361</t>
+          <t>4752</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>28749280</t>
+          <t>38711610</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>㊥老船⛵⛵</t>
+          <t>心灵有为</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>5843</t>
+          <t>6243</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>7730</t>
+          <t>2566</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>13738844</t>
+          <t>43800641</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>"Chen Hao"</t>
+          <t>㊥蛋蛋大</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>5382</t>
+          <t>6637</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>9735</t>
+          <t>4037</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>43812707</t>
+          <t>44955827</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>bbtt</t>
+          <t>丶小阿狸丿</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>5145</t>
+          <t>6345</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>10351</t>
+          <t>48730</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>42434117</t>
+          <t>45967307</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>㊥有双飞鸟</t>
+          <t>Ricky</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>5085</t>
+          <t>3098</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>10652</t>
+          <t>2220</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>49710892</t>
+          <t>46422609</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>MMMMMMM</t>
+          <t>㊥林天大大神</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>5057</t>
+          <t>6721</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>11805</t>
+          <t>12131</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>53060417</t>
+          <t>47146736</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>㊥老纳信耶稣</t>
+          <t>"HK 品瑜"</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4959</t>
+          <t>5239</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>12756</t>
+          <t>1033</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>53520939</t>
+          <t>47928278</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>㊥虎哥tiger</t>
+          <t>"落日幻影 哈哈哈"</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>4876</t>
+          <t>7088</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>16346</t>
+          <t>46099</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4756174</t>
+          <t>29565</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>純希です</t>
+          <t>"aK.j Zhong ㊥"</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1739,24 +1739,24 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4590</t>
+          <t>3231</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>17081</t>
+          <t>50374</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>31495601</t>
+          <t>68132</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>陈晓军</t>
+          <t>"㊖TW9 百媚生"</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1766,24 +1766,24 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>4541</t>
+          <t>3019</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>17253</t>
+          <t>41008</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>54698813</t>
+          <t>1550355</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>閃亮唐老鴨</t>
+          <t>"皓茵 世界"</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1793,24 +1793,24 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>4531</t>
+          <t>3450</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>40311</t>
+          <t>5400</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>55769051</t>
+          <t>4493731</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>㊥叮叮当.</t>
+          <t>Player-1527362</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1820,24 +1820,24 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>3358</t>
+          <t>6136</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>537</t>
+          <t>19758</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8741713</t>
+          <t>4756174</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t xml:space="preserve">㊥大咖玩家ky </t>
+          <t>純希です</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1847,24 +1847,24 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>6706</t>
+          <t>4610</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>576</t>
+          <t>16966</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>20199374</t>
+          <t>6809364</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>RuanFan</t>
+          <t>"Scorp IP"</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1874,24 +1874,24 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>6690</t>
+          <t>4774</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>870</t>
+          <t>8007</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>3946814</t>
+          <t>7852598</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>"小瑩 潘"</t>
+          <t>seiji</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1901,24 +1901,24 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>6588</t>
+          <t>5691</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2978</t>
+          <t>14926</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>46422609</t>
+          <t>8057001</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>㊥林天大大神</t>
+          <t>㊥兵者诡道也</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1928,24 +1928,24 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>6067</t>
+          <t>4944</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>3568</t>
+          <t>21416</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>26588375</t>
+          <t>9212603</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>kusipao</t>
+          <t>KymBaoNgoc</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1955,24 +1955,24 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>5969</t>
+          <t>4529</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>4726</t>
+          <t>20800</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16206490</t>
+          <t>11548491</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>㊥Godcys</t>
+          <t>"Thương VNG"</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1982,24 +1982,24 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>5798</t>
+          <t>4559</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>4901</t>
+          <t>9188</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>9541747</t>
+          <t>11582001</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>豹子头林冲</t>
+          <t>iMinatoX4</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2009,24 +2009,24 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>5775</t>
+          <t>5514</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>5280</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>38711610</t>
+          <t>12639656</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>心灵有为</t>
+          <t>"wu huang"</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2036,24 +2036,24 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>5723</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>5899</t>
+          <t>8246</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>4493731</t>
+          <t>13738844</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Player-1527362</t>
+          <t>"Chen Hao"</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2063,24 +2063,24 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>5638</t>
+          <t>5646</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7250</t>
+          <t>32504</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7025661</t>
+          <t>14110169</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>"F ᶻᵍˣ"</t>
+          <t>"Pasiony CANQ"</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2090,24 +2090,24 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>5446</t>
+          <t>3869</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>8720</t>
+          <t>16475</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>47131129</t>
+          <t>20766468</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>NAM</t>
+          <t>Player-6160225</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2117,24 +2117,24 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>5251</t>
+          <t>4812</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>8759</t>
+          <t>40961</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7852598</t>
+          <t>22161051</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>seiji</t>
+          <t>Botz5</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2144,24 +2144,24 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>5246</t>
+          <t>3452</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>9499</t>
+          <t>10688</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>11582001</t>
+          <t>22885399</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>iMinatoX4</t>
+          <t>余文琪</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -2171,24 +2171,24 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>5169</t>
+          <t>5350</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>10321</t>
+          <t>2704</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>22885399</t>
+          <t>26588375</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>余文琪</t>
+          <t>kusipao</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2198,24 +2198,24 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>5088</t>
+          <t>6605</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>14974</t>
+          <t>16831</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>56133764</t>
+          <t>31495601</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ustcarter</t>
+          <t>陈晓军</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2225,24 +2225,24 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>4690</t>
+          <t>4785</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>16258</t>
+          <t>17454</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>6809364</t>
+          <t>32316256</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>"Scorp IP"</t>
+          <t>"秋の風 .."</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2252,24 +2252,24 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>4596</t>
+          <t>4755</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>16907</t>
+          <t>16116</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>20766468</t>
+          <t>37861953</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Player-6160225</t>
+          <t>"Durex ๑• . •๑"</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2279,24 +2279,24 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>4552</t>
+          <t>4840</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>18011</t>
+          <t>23531</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>11548491</t>
+          <t>38561634</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>"Thương VNG"</t>
+          <t>"Ambrose PT"</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2306,24 +2306,24 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>4487</t>
+          <t>4370</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>18786</t>
+          <t>18384</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8057001</t>
+          <t>38809086</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>㊥兵者诡道也</t>
+          <t>Kouenᶻᵍˣ</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2333,24 +2333,24 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>4440</t>
+          <t>4684</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>20187</t>
+          <t>17898</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>38995116</t>
+          <t>38893233</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>"Ramesh Pavai Nam"</t>
+          <t>"快乐 二哈"</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2360,24 +2360,24 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>4360</t>
+          <t>4712</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>21320</t>
+          <t>21793</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9212603</t>
+          <t>38995116</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>KymBaoNgoc</t>
+          <t>"Ramesh Pavai Nam"</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2387,24 +2387,24 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>4292</t>
+          <t>4512</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>21682</t>
+          <t>9504</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>38893233</t>
+          <t>42434117</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>"快乐 二哈"</t>
+          <t>㊥有双飞鸟</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -2414,24 +2414,24 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>4272</t>
+          <t>5478</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>24445</t>
+          <t>10669</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>38561634</t>
+          <t>43812707</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>"Ambrose PT"</t>
+          <t>bbtt</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -2441,24 +2441,24 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>4102</t>
+          <t>5360</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>25749</t>
+          <t>7888</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>32316256</t>
+          <t>47131129</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>"秋の風 .."</t>
+          <t>NAM</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>4025</t>
+          <t>5713</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>36925</t>
+          <t>68302</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>22161051</t>
+          <t>47758619</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Botz5</t>
+          <t>"㊥ Moon ㊥"</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2495,24 +2495,24 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>3502</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>37016</t>
+          <t>12553</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>55860890</t>
+          <t>49710892</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>㊥Ethan</t>
+          <t>MMMMMMM</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2522,24 +2522,24 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>3498</t>
+          <t>5207</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>37574</t>
+          <t>10620</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>56573048</t>
+          <t>53060417</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Xiaotian</t>
+          <t>㊥老纳信耶稣</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2549,24 +2549,24 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>3475</t>
+          <t>5364</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>38929</t>
+          <t>12864</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>54714516</t>
+          <t>53520939</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>ёмιいч</t>
+          <t>㊥虎哥tiger</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2576,24 +2576,24 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>3417</t>
+          <t>5203</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>40273</t>
+          <t>16101</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>1550355</t>
+          <t>54698813</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>"皓茵 世界"</t>
+          <t>閃亮唐老鴨</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2603,24 +2603,24 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>3360</t>
+          <t>4841</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>47079</t>
+          <t>41018</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>56500325</t>
+          <t>54714516</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>haruharuyukizg9735</t>
+          <t>ёмιいч</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2630,24 +2630,24 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>3070</t>
+          <t>3449</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>47910</t>
+          <t>29239</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>14110169</t>
+          <t>55769051</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>"Pasiony CANQ"</t>
+          <t>㊥叮叮当.</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2657,24 +2657,24 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>3036</t>
+          <t>4015</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>51083</t>
+          <t>33452</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>29565</t>
+          <t>55860890</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>"aK.j Zhong ㊥"</t>
+          <t>㊥Ethan</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2684,24 +2684,24 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>2907</t>
+          <t>3826</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>51246</t>
+          <t>13632</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>68132</t>
+          <t>56133764</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>"㊖TW9 百媚生"</t>
+          <t>ustcarter</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2711,24 +2711,24 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>2900</t>
+          <t>5073</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>51913</t>
+          <t>49081</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>57813281</t>
+          <t>56500325</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>XAUEN</t>
+          <t>haruharuyukizg9735</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2738,24 +2738,24 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>2876</t>
+          <t>3082</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>52281</t>
+          <t>39804</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>58203298</t>
+          <t>56573048</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>权旨qua</t>
+          <t>Xiaotian</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2765,24 +2765,24 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>2863</t>
+          <t>3503</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>66792</t>
+          <t>54168</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>47758619</t>
+          <t>57813281</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>"㊥ Moon ㊥"</t>
+          <t>XAUEN</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2792,24 +2792,24 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2861</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>54909</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>12639656</t>
+          <t>58203298</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>"wu huang"</t>
+          <t>权旨qua</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2819,24 +2819,24 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2833</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>53849</t>
+          <t>77337</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>44378757</t>
+          <t>1222440</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
+          <t>"Sneaky Ninja Panda"</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2846,24 +2846,24 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>2808</t>
+          <t>2309</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>17348</t>
+          <t>50639</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>25163202</t>
+          <t>1304123</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>"sam yang"</t>
+          <t>Cccccccccccc</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2873,24 +2873,24 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>4527</t>
+          <t>3008</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>17889</t>
+          <t>43438</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>31134300</t>
+          <t>3391765</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>McMaX</t>
+          <t>马er</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2900,24 +2900,24 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>3344</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>24969</t>
+          <t>57867</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>25479797</t>
+          <t>5367482</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>"Mohamed Alnaqbi"</t>
+          <t>Ігор</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2927,24 +2927,24 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>4071</t>
+          <t>2735</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>25771</t>
+          <t>50827</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>44708798</t>
+          <t>9718882</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>"㊥ mythgod"</t>
+          <t>小霸王2021</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2954,24 +2954,24 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>4024</t>
+          <t>3000</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>25802</t>
+          <t>58652</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>54778421</t>
+          <t>11645391</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Emma</t>
+          <t>"omar omar"</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2981,24 +2981,24 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>4022</t>
+          <t>2712</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>25937</t>
+          <t>80903</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>37069173</t>
+          <t>15436348</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>詹toniii</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3008,24 +3008,24 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>4016</t>
+          <t>2236</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>29334</t>
+          <t>26831</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>28855852</t>
+          <t>18082891</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>tiger</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3035,24 +3035,24 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>3846</t>
+          <t>4144</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>60780</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>54588689</t>
+          <t>20372140</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>㊥墨衍枫迹☜</t>
+          <t>Player-20372140</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3062,24 +3062,24 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2653</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>1420</t>
+          <t>18301</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>29211638</t>
+          <t>25163202</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>"㊥ PhononDisperse"</t>
+          <t>"sam yang"</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3089,24 +3089,24 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>6429</t>
+          <t>4688</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>28782</t>
+          <t>25847</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>48634530</t>
+          <t>25479797</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>leezhenrui</t>
+          <t>"Mohamed Alnaqbi"</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -3116,24 +3116,24 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>3871</t>
+          <t>4206</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>29943</t>
+          <t>31961</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>18082891</t>
+          <t>28855852</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>tiger</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -3143,24 +3143,24 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>3817</t>
+          <t>3892</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>29930</t>
+          <t>18610</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>54085771</t>
+          <t>31134300</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>㊥Matthieu</t>
+          <t>McMaX</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3170,24 +3170,24 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>3817</t>
+          <t>4671</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>30753</t>
+          <t>26158</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>56700848</t>
+          <t>37069173</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>工口漫画老师</t>
+          <t>詹toniii</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3197,24 +3197,24 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>3780</t>
+          <t>4187</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>33473</t>
+          <t>75100</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>47459684</t>
+          <t>38994054</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>㊥阿闹切克闹</t>
+          <t>chengnan</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -3224,24 +3224,24 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>3657</t>
+          <t>2362</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>33752</t>
+          <t>59710</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>46289694</t>
+          <t>43281368</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>㊥Vincent</t>
+          <t>xhs2763</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -3251,24 +3251,24 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>3645</t>
+          <t>2681</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>38846</t>
+          <t>55609</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>56379103</t>
+          <t>44378757</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Globalking</t>
+          <t>"NᵉᵗʰᵉʳDʳⁱᶠᵗᵉʳ ㊥"</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3278,24 +3278,24 @@
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>3420</t>
+          <t>2808</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>39063</t>
+          <t>27775</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>56585361</t>
+          <t>44708798</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>"㊥ go策划我要ali"</t>
+          <t>"㊥ mythgod"</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3305,24 +3305,24 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>3411</t>
+          <t>4090</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>40810</t>
+          <t>32580</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>52997727</t>
+          <t>46289694</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>㊥Vincent</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -3332,24 +3332,24 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>3338</t>
+          <t>3865</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>40935</t>
+          <t>46153</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>3391765</t>
+          <t>47227626</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>马er</t>
+          <t>Player-47227626</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -3359,24 +3359,24 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>3333</t>
+          <t>3228</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>41270</t>
+          <t>44725</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>56732705</t>
+          <t>47430231</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>时间温柔皆遗憾</t>
+          <t>Kentantrino</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -3386,24 +3386,24 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>3319</t>
+          <t>3291</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>44886</t>
+          <t>33752</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>47430231</t>
+          <t>47459684</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Kentantrino</t>
+          <t>㊥阿闹切克闹</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -3413,24 +3413,24 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>3167</t>
+          <t>3814</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>45712</t>
+          <t>29819</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>55634661</t>
+          <t>48634530</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>leezhenrui</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3440,24 +3440,24 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>3130</t>
+          <t>3991</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>47522</t>
+          <t>66712</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>58615925</t>
+          <t>52792063</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>齐天的大圣</t>
+          <t>"Tramaine Dowlen"</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -3467,24 +3467,24 @@
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>3052</t>
+          <t>2526</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>48752</t>
+          <t>39450</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>47227626</t>
+          <t>52997727</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Player-47227626</t>
+          <t>larios</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -3494,24 +3494,24 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>3001</t>
+          <t>3519</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>52192</t>
+          <t>27771</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>1304123</t>
+          <t>54085771</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Cccccccccccc</t>
+          <t>㊥Matthieu</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -3521,24 +3521,24 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>2867</t>
+          <t>4091</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>55065</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>5367482</t>
+          <t>54588689</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Ігор</t>
+          <t>㊥墨衍枫迹☜</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -3548,24 +3548,24 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>55687</t>
+          <t>25374</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>58641574</t>
+          <t>54778421</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Player-58641574</t>
+          <t>Emma</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -3575,14 +3575,14 @@
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>2748</t>
+          <t>4234</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>57525</t>
+          <t>50624</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -3602,24 +3602,24 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>2695</t>
+          <t>3008</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>57958</t>
+          <t>45262</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>11645391</t>
+          <t>55634661</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>"omar omar"</t>
+          <t>Opalus</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -3629,24 +3629,24 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>2683</t>
+          <t>3267</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>58047</t>
+          <t>60727</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>43281368</t>
+          <t>55810157</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>xhs2763</t>
+          <t>Beard</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -3656,24 +3656,24 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>2680</t>
+          <t>2654</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>61346</t>
+          <t>39614</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>9718882</t>
+          <t>56379103</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>小霸王2021</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
@@ -3683,24 +3683,24 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>2599</t>
+          <t>3512</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>62307</t>
+          <t>39888</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>55810157</t>
+          <t>56585361</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Beard</t>
+          <t>"㊥ go策划我要ali"</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -3710,24 +3710,24 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>2579</t>
+          <t>3499</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>66253</t>
+          <t>30852</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>52792063</t>
+          <t>56700848</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>"Tramaine Dowlen"</t>
+          <t>工口漫画老师</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -3737,24 +3737,24 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>2508</t>
+          <t>3940</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>67174</t>
+          <t>38136</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>1222440</t>
+          <t>56732705</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>"Sneaky Ninja Panda"</t>
+          <t>时间温柔皆遗憾</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -3764,14 +3764,14 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>2498</t>
+          <t>3583</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>68254</t>
+          <t>66021</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3791,24 +3791,24 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>2482</t>
+          <t>2537</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>70822</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>20372140</t>
+          <t>57556179</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Player-20372140</t>
+          <t>特战新生代英雄</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3818,24 +3818,24 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>2430</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>73329</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>38994054</t>
+          <t>58340439</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>chengnan</t>
+          <t>70qilin</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3845,24 +3845,24 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>2369</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>78827</t>
+          <t>50515</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>15436348</t>
+          <t>58408326</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>"Killer Bee"</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3872,24 +3872,24 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>2239</t>
+          <t>3013</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>46067</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>57556179</t>
+          <t>58615925</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>特战新生代英雄</t>
+          <t>齐天的大圣</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3899,24 +3899,24 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3232</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>55497</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>58340439</t>
+          <t>58641574</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>70qilin</t>
+          <t>Player-58641574鱼</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3926,14 +3926,14 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2811</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>53658</t>
+          <t>47379</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>2815</t>
+          <t>3168</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>45720</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>46248210</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>Ajay</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,24 +3980,24 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>3130</t>
+          <t>1218</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>45866</t>
+          <t>79079</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>47533851</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>Bibek</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,24 +4007,24 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>3123</t>
+          <t>2271</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>59585</t>
+          <t>47408</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4034,14 +4034,14 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>2640</t>
+          <t>3166</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>64868</t>
+          <t>66453</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -4068,17 +4068,17 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>70880</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>50742014</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>"Aditya Naik"</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4088,24 +4088,24 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>2428</t>
+          <t>997</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>74488</t>
+          <t>61997</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>58739336</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Player-58739336</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4115,24 +4115,24 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>2338</t>
+          <t>2623</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>78098</t>
+          <t>47038</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>47533851</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Bibek</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4142,24 +4142,24 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>2253</t>
+          <t>3186</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>100351</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>58689512</t>
+          <t>57339836</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Player-58689512</t>
+          <t>Player-57339836</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4169,24 +4169,24 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>1751</t>
+          <t>1100</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>108926</t>
+          <t>69563</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>58644547</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>RotaryPreparation39</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,24 +4196,24 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>1597</t>
+          <t>2485</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>110118</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>58635041</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>Player-58635041</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,24 +4223,24 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>1580</t>
+          <t>1500</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>118174</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>58635041</t>
+          <t>58644547</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Player-58635041</t>
+          <t>RotaryPreparation39</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4250,24 +4250,24 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1613</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>128746</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>58739866</t>
+          <t>58689512</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Player-58739866</t>
+          <t>Player-58689512</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4277,24 +4277,24 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>1408</t>
+          <t>1755</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>156418</t>
+          <t>77253</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>46248210</t>
+          <t>58739336</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Ajay</t>
+          <t>Player-58739336</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4304,24 +4304,24 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>1199</t>
+          <t>2310</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>168783</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>57339836</t>
+          <t>58739866</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Player-57339836</t>
+          <t>Player-58739866</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4331,24 +4331,24 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>1697</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>268435</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>50742014</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>"Aditya Naik"</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4358,24 +4358,24 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>998</t>
+          <t>1619</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>46679</t>
+          <t>6752</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>41848598</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>国家一级保护沙雕</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -4385,24 +4385,24 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>3088</t>
+          <t>5979</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>6178</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -4412,24 +4412,24 @@
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>5603</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>45261</t>
+          <t>67421</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -4439,24 +4439,24 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>3150</t>
+          <t>2514</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>66704</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -4466,24 +4466,24 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>46711</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -4493,24 +4493,24 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3202</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>28624723</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>"Woody Shade"</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -4527,17 +4527,17 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>47854</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -4547,7 +4547,7 @@
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3143</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-10-08 11:31:03
</commit_message>
<xml_diff>
--- a/Season_Trophies/83.xlsx
+++ b/Season_Trophies/83.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E155"/>
+  <dimension ref="A1:E187"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3933,17 +3933,17 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>47384</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>41849539</t>
+          <t>10637292</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>三号馆馆主</t>
+          <t>ᴱᵁᴿWacheSimonᴵᵀᴬ</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>3168</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>61997</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>46248210</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Ajay</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,24 +3980,24 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>1218</t>
+          <t>2623</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>79079</t>
+          <t>47037</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>47533851</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Bibek</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,24 +4007,24 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>2271</t>
+          <t>3186</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>47413</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>47622456</t>
+          <t>57339836</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>伊恩</t>
+          <t>Player-57339836</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4034,24 +4034,24 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>3166</t>
+          <t>1100</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>66453</t>
+          <t>69563</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>49553719</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>"Oreo Captain Sir"</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2530</t>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -4073,12 +4073,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>50742014</t>
+          <t>58635041</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>"Aditya Naik"</t>
+          <t>Player-58635041</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4088,24 +4088,24 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>997</t>
+          <t>1500</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>61997</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>58644547</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>RotaryPreparation39</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4115,24 +4115,24 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>2623</t>
+          <t>1613</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>47037</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>58689512</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>Player-58689512</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4142,24 +4142,24 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>3186</t>
+          <t>1755</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>77255</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>57339836</t>
+          <t>58739336</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Player-57339836</t>
+          <t>Player-58739336</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4169,24 +4169,24 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>2310</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>69563</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>58739866</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>Player-58739866</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>1697</t>
         </is>
       </c>
     </row>
@@ -4208,12 +4208,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>58635041</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Player-58635041</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,24 +4223,20 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>1619</t>
         </is>
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A144" t="inlineStr"/>
       <c r="B144" t="inlineStr">
         <is>
-          <t>58644547</t>
+          <t>"Clan Level"</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>RotaryPreparation39</t>
+          <t>26</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4250,24 +4246,20 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>1613</t>
+          <t>Members</t>
         </is>
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="A145" t="inlineStr"/>
       <c r="B145" t="inlineStr">
         <is>
-          <t>58689512</t>
+          <t>9807776</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Player-58689512</t>
+          <t>"EUR AlterBeast"</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4277,24 +4269,24 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>1755</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>77255</t>
+          <t>12199</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>58739336</t>
+          <t>4305318</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Player-58739336</t>
+          <t>"EUR Gio Vanni"</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4304,24 +4296,24 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>2310</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>11691</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>58739866</t>
+          <t>45765287</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Player-58739866</t>
+          <t>"EUR Koppie"</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4331,24 +4323,24 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>1697</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>17015</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>17142449</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>"EUR PiPP8TTo"</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4358,164 +4350,164 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>1619</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>6700</t>
+          <t>14108</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>6010122</t>
+          <t>31825557</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>"Edward Peng"</t>
+          <t>"EUR  FALCO  ITA"</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>5979</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>13583</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>8850180</t>
+          <t>3395158</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>30624300</t>
+          <t>"EUR Rotonda"</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>67421</t>
+          <t>7807</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>9195340</t>
+          <t>8572291</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Namllllllik</t>
+          <t>"EUR Bassie"</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>2514</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>9266</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>12648101</t>
+          <t>57009371</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>"player 198827"</t>
+          <t>:Zam:</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>46712</t>
+          <t>17923</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>15755724</t>
+          <t>10991123</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>"Last Good"</t>
+          <t>"EUR smadott"</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>3202</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>999999</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>28624723</t>
+          <t>3524101</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>"Woody Shade"</t>
+          <t>"EUR Mirko ITA"</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Chinese</t>
+          <t>三馆</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -4527,25 +4519,889 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>10117616</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>EUR.giuseppe.</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>11166772</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>ᴱᵁᴿTheScotsman</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>10501718</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>HappyRiderᴱᵁᴿ</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>4488786</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>"ᴱᵁᴿ Sami ᴿᴼᴹ"</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>23672709</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>"EUR Jelle L"</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>5871525</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>"EUR ITA - Lucio"</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>35506178</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>"EUR ITA Davide"</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>30708890</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>"ᴱᵁᴿ GruttePierᶰᶫ"</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>25697696</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>"Eur MANDRAKE"</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>7322925</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>"Eur Jack ᴵᵀᴬ"</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>8866548</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>"EUR theDarkie"</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>11069212</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>"EUR DFI Mobywan"</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>3408905</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>"Mr Bean"</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>14728103</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>"Cioffi Luigi ITA"</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>27157062</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>"EUR Mangusta ᴵᵀᴬ"</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>31173607</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>BoccinoPlanarITA</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>2918936</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>CozMyn</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>25333088</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>EUR-Florin</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>20597185</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>EUR-DARIO.Bᴵᵀᴬ</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>20906662</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>EUR-MOICANO-IRON</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>20549488</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>"Novis Somniumᴱᵁᴿ"</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>17169547</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>Sampler</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>36497324</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>"Mark Layton EUR4"</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>31363087</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>"ITA Nino ZX21"</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>40854051</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>Seriously</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>999999</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>8947174</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>Grizzly</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>6700</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>6010122</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>"Edward Peng"</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>5979</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>8850180</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>30624300</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>67421</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>9195340</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>Namllllllik</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>2514</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>12648101</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>"player 198827"</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>46712</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>15755724</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>"Last Good"</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>3202</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>28624723</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>"Woody Shade"</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Chinese</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
           <t>47857</t>
         </is>
       </c>
-      <c r="B155" t="inlineStr">
+      <c r="B187" t="inlineStr">
         <is>
           <t>41848598</t>
         </is>
       </c>
-      <c r="C155" t="inlineStr">
+      <c r="C187" t="inlineStr">
         <is>
           <t>国家一级保护沙雕</t>
         </is>
       </c>
-      <c r="D155" t="inlineStr">
+      <c r="D187" t="inlineStr">
         <is>
           <t>Chinese</t>
         </is>
       </c>
-      <c r="E155" t="inlineStr">
+      <c r="E187" t="inlineStr">
         <is>
           <t>3143</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-10-09 11:31:02
</commit_message>
<xml_diff>
--- a/Season_Trophies/83.xlsx
+++ b/Season_Trophies/83.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E187"/>
+  <dimension ref="A1:E155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3933,17 +3933,17 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>47384</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>10637292</t>
+          <t>41849539</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>ᴱᵁᴿWacheSimonᴵᵀᴬ</t>
+          <t>三号馆馆主</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3953,24 +3953,24 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3168</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>61997</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>55210350</t>
+          <t>46248210</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>一个过客而已</t>
+          <t>Ajay</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3980,24 +3980,24 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>2623</t>
+          <t>1218</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>47037</t>
+          <t>79079</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>56241637</t>
+          <t>47533851</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Player-14day</t>
+          <t>Bibek</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4007,24 +4007,24 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>3186</t>
+          <t>2271</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>47413</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>57339836</t>
+          <t>47622456</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Player-57339836</t>
+          <t>伊恩</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -4034,24 +4034,24 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>1100</t>
+          <t>3166</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>69563</t>
+          <t>66453</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>58572199</t>
+          <t>49553719</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>你干嘛～哎呦～</t>
+          <t>"Oreo Captain Sir"</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -4073,12 +4073,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>58635041</t>
+          <t>50742014</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Player-58635041</t>
+          <t>"Aditya Naik"</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -4088,24 +4088,24 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>1500</t>
+          <t>997</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>61997</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>58644547</t>
+          <t>55210350</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>RotaryPreparation39</t>
+          <t>一个过客而已</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -4115,24 +4115,24 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>1613</t>
+          <t>2623</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>47037</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>58689512</t>
+          <t>56241637</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Player-58689512</t>
+          <t>Player-14day</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -4142,24 +4142,24 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>1755</t>
+          <t>3186</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>77255</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>58739336</t>
+          <t>57339836</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Player-58739336</t>
+          <t>Player-57339836</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -4169,24 +4169,24 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>2310</t>
+          <t>1100</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>69563</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>58739866</t>
+          <t>58572199</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Player-58739866</t>
+          <t>你干嘛～哎呦～</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>1697</t>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -4208,12 +4208,12 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>58766144</t>
+          <t>58635041</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>EquablePrecedence38</t>
+          <t>Player-58635041</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -4223,20 +4223,24 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>1619</t>
+          <t>1500</t>
         </is>
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr"/>
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>"Clan Level"</t>
+          <t>58644547</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>RotaryPreparation39</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -4246,20 +4250,24 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Members</t>
+          <t>1613</t>
         </is>
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr"/>
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>9807776</t>
+          <t>58689512</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>"EUR AlterBeast"</t>
+          <t>Player-58689512</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -4269,24 +4277,24 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>1755</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>12199</t>
+          <t>77255</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>4305318</t>
+          <t>58739336</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>"EUR Gio Vanni"</t>
+          <t>Player-58739336</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -4296,24 +4304,24 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2310</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>11691</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>45765287</t>
+          <t>58739866</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>"EUR Koppie"</t>
+          <t>Player-58739866</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -4323,24 +4331,24 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>1697</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>17015</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>17142449</t>
+          <t>58766144</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>"EUR PiPP8TTo"</t>
+          <t>EquablePrecedence38</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -4350,164 +4358,164 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>1619</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>14108</t>
+          <t>6700</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>31825557</t>
+          <t>6010122</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>"EUR  FALCO  ITA"</t>
+          <t>"Edward Peng"</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>5979</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>13583</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>3395158</t>
+          <t>8850180</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>"EUR Rotonda"</t>
+          <t>30624300</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>7807</t>
+          <t>67421</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>8572291</t>
+          <t>9195340</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>"EUR Bassie"</t>
+          <t>Namllllllik</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2514</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>9266</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>57009371</t>
+          <t>12648101</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>:Zam:</t>
+          <t>"player 198827"</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>17923</t>
+          <t>46712</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>10991123</t>
+          <t>15755724</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>"EUR smadott"</t>
+          <t>"Last Good"</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>3202</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>3524101</t>
+          <t>28624723</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>"EUR Mirko ITA"</t>
+          <t>"Woody Shade"</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -4519,889 +4527,25 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>999999</t>
+          <t>47857</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>10117616</t>
+          <t>41848598</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>EUR.giuseppe.</t>
+          <t>国家一级保护沙雕</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>Chinese</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>11166772</t>
-        </is>
-      </c>
-      <c r="C156" t="inlineStr">
-        <is>
-          <t>ᴱᵁᴿTheScotsman</t>
-        </is>
-      </c>
-      <c r="D156" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E156" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr">
-        <is>
-          <t>10501718</t>
-        </is>
-      </c>
-      <c r="C157" t="inlineStr">
-        <is>
-          <t>HappyRiderᴱᵁᴿ</t>
-        </is>
-      </c>
-      <c r="D157" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E157" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>4488786</t>
-        </is>
-      </c>
-      <c r="C158" t="inlineStr">
-        <is>
-          <t>"ᴱᵁᴿ Sami ᴿᴼᴹ"</t>
-        </is>
-      </c>
-      <c r="D158" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E158" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>23672709</t>
-        </is>
-      </c>
-      <c r="C159" t="inlineStr">
-        <is>
-          <t>"EUR Jelle L"</t>
-        </is>
-      </c>
-      <c r="D159" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E159" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr">
-        <is>
-          <t>5871525</t>
-        </is>
-      </c>
-      <c r="C160" t="inlineStr">
-        <is>
-          <t>"EUR ITA - Lucio"</t>
-        </is>
-      </c>
-      <c r="D160" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E160" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr">
-        <is>
-          <t>35506178</t>
-        </is>
-      </c>
-      <c r="C161" t="inlineStr">
-        <is>
-          <t>"EUR ITA Davide"</t>
-        </is>
-      </c>
-      <c r="D161" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E161" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr">
-        <is>
-          <t>30708890</t>
-        </is>
-      </c>
-      <c r="C162" t="inlineStr">
-        <is>
-          <t>"ᴱᵁᴿ GruttePierᶰᶫ"</t>
-        </is>
-      </c>
-      <c r="D162" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E162" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr">
-        <is>
-          <t>25697696</t>
-        </is>
-      </c>
-      <c r="C163" t="inlineStr">
-        <is>
-          <t>"Eur MANDRAKE"</t>
-        </is>
-      </c>
-      <c r="D163" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E163" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>7322925</t>
-        </is>
-      </c>
-      <c r="C164" t="inlineStr">
-        <is>
-          <t>"Eur Jack ᴵᵀᴬ"</t>
-        </is>
-      </c>
-      <c r="D164" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E164" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>8866548</t>
-        </is>
-      </c>
-      <c r="C165" t="inlineStr">
-        <is>
-          <t>"EUR theDarkie"</t>
-        </is>
-      </c>
-      <c r="D165" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E165" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>11069212</t>
-        </is>
-      </c>
-      <c r="C166" t="inlineStr">
-        <is>
-          <t>"EUR DFI Mobywan"</t>
-        </is>
-      </c>
-      <c r="D166" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E166" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>3408905</t>
-        </is>
-      </c>
-      <c r="C167" t="inlineStr">
-        <is>
-          <t>"Mr Bean"</t>
-        </is>
-      </c>
-      <c r="D167" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E167" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>14728103</t>
-        </is>
-      </c>
-      <c r="C168" t="inlineStr">
-        <is>
-          <t>"Cioffi Luigi ITA"</t>
-        </is>
-      </c>
-      <c r="D168" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>27157062</t>
-        </is>
-      </c>
-      <c r="C169" t="inlineStr">
-        <is>
-          <t>"EUR Mangusta ᴵᵀᴬ"</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E169" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr">
-        <is>
-          <t>31173607</t>
-        </is>
-      </c>
-      <c r="C170" t="inlineStr">
-        <is>
-          <t>BoccinoPlanarITA</t>
-        </is>
-      </c>
-      <c r="D170" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E170" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>2918936</t>
-        </is>
-      </c>
-      <c r="C171" t="inlineStr">
-        <is>
-          <t>CozMyn</t>
-        </is>
-      </c>
-      <c r="D171" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E171" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>25333088</t>
-        </is>
-      </c>
-      <c r="C172" t="inlineStr">
-        <is>
-          <t>EUR-Florin</t>
-        </is>
-      </c>
-      <c r="D172" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E172" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>20597185</t>
-        </is>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>EUR-DARIO.Bᴵᵀᴬ</t>
-        </is>
-      </c>
-      <c r="D173" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E173" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>20906662</t>
-        </is>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>EUR-MOICANO-IRON</t>
-        </is>
-      </c>
-      <c r="D174" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E174" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>20549488</t>
-        </is>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>"Novis Somniumᴱᵁᴿ"</t>
-        </is>
-      </c>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E175" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>17169547</t>
-        </is>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>Sampler</t>
-        </is>
-      </c>
-      <c r="D176" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E176" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>36497324</t>
-        </is>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>"Mark Layton EUR4"</t>
-        </is>
-      </c>
-      <c r="D177" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E177" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>31363087</t>
-        </is>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>"ITA Nino ZX21"</t>
-        </is>
-      </c>
-      <c r="D178" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E178" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B179" t="inlineStr">
-        <is>
-          <t>40854051</t>
-        </is>
-      </c>
-      <c r="C179" t="inlineStr">
-        <is>
-          <t>Seriously</t>
-        </is>
-      </c>
-      <c r="D179" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E179" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>999999</t>
-        </is>
-      </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>8947174</t>
-        </is>
-      </c>
-      <c r="C180" t="inlineStr">
-        <is>
-          <t>Grizzly</t>
-        </is>
-      </c>
-      <c r="D180" t="inlineStr">
-        <is>
-          <t>三馆</t>
-        </is>
-      </c>
-      <c r="E180" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>6700</t>
-        </is>
-      </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>6010122</t>
-        </is>
-      </c>
-      <c r="C181" t="inlineStr">
-        <is>
-          <t>"Edward Peng"</t>
-        </is>
-      </c>
-      <c r="D181" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E181" t="inlineStr">
-        <is>
-          <t>5979</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>8850180</t>
-        </is>
-      </c>
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>30624300</t>
-        </is>
-      </c>
-      <c r="D182" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E182" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>67421</t>
-        </is>
-      </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>9195340</t>
-        </is>
-      </c>
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>Namllllllik</t>
-        </is>
-      </c>
-      <c r="D183" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E183" t="inlineStr">
-        <is>
-          <t>2514</t>
-        </is>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>12648101</t>
-        </is>
-      </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>"player 198827"</t>
-        </is>
-      </c>
-      <c r="D184" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E184" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>46712</t>
-        </is>
-      </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>15755724</t>
-        </is>
-      </c>
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>"Last Good"</t>
-        </is>
-      </c>
-      <c r="D185" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E185" t="inlineStr">
-        <is>
-          <t>3202</t>
-        </is>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>28624723</t>
-        </is>
-      </c>
-      <c r="C186" t="inlineStr">
-        <is>
-          <t>"Woody Shade"</t>
-        </is>
-      </c>
-      <c r="D186" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E186" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>47857</t>
-        </is>
-      </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>41848598</t>
-        </is>
-      </c>
-      <c r="C187" t="inlineStr">
-        <is>
-          <t>国家一级保护沙雕</t>
-        </is>
-      </c>
-      <c r="D187" t="inlineStr">
-        <is>
-          <t>Chinese</t>
-        </is>
-      </c>
-      <c r="E187" t="inlineStr">
         <is>
           <t>3143</t>
         </is>

</xml_diff>